<commit_message>
Better Gene Inheritance 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Better Gene Inheritance - 3046776238/Better Gene Inheritance - 3046776238.xlsx
+++ b/Data/Better Gene Inheritance - 3046776238/Better Gene Inheritance - 3046776238.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zilrt\Desktop\RimworldExtractor-Standard\Better Gene Inheritance - 3046776238\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\trans\Better Gene Inheritance - 3046776238\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB6ABD6-7A9A-4525-B2F8-7CAD48FF6608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E365E3AF-5D5B-4E39-BA47-B7CB32C8B797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -52,6 +52,9 @@
     <t>Dominant Genes</t>
   </si>
   <si>
+    <t>우성 유전자</t>
+  </si>
+  <si>
     <t>GeneDef+BGI_DominantGenes.description</t>
   </si>
   <si>
@@ -70,6 +73,9 @@
     <t>Recessive Genes</t>
   </si>
   <si>
+    <t>열성 유전자</t>
+  </si>
+  <si>
     <t>GeneDef+BGI_RecessiveGenes.description</t>
   </si>
   <si>
@@ -92,66 +98,6 @@
   </si>
   <si>
     <t>Keyed+BGI_InheritArchite</t>
-  </si>
-  <si>
-    <t>BGI_InheritArchite</t>
-  </si>
-  <si>
-    <t>Archite Genes are inheritable.</t>
-  </si>
-  <si>
-    <t>Keyed+BGI_InheritXeno</t>
-  </si>
-  <si>
-    <t>BGI_InheritXeno</t>
-  </si>
-  <si>
-    <t>Xenogenes can be inherited along with the endogenes.</t>
-  </si>
-  <si>
-    <t>Keyed+BGInheritance</t>
-  </si>
-  <si>
-    <t>BGInheritance</t>
-  </si>
-  <si>
-    <t>Better Gene Inheritance</t>
-  </si>
-  <si>
-    <t>Keyed+BGI_MetabolismLimit</t>
-  </si>
-  <si>
-    <t>BGI_MetabolismLimit</t>
-  </si>
-  <si>
-    <t>Lowest permitted metabolism</t>
-  </si>
-  <si>
-    <t>우성 유전자</t>
-  </si>
-  <si>
-    <t>이 유전자를 가진 자는 자손에게 모든 유전자를 전달하며, 파트너의 유전자는 무시됩니다. 단, 파트너도 이 유전자를 가진 경우는 예외입니다.</t>
-  </si>
-  <si>
-    <t>열성 유전자</t>
-  </si>
-  <si>
-    <t>이 유전자를 가진 자는 자손에게 아무 유전자도 전달하지 않으며, 파트너의 유전자만 받습니다. 단, 파트너도 이 유전자를 가진 경우는 예외입니다.</t>
-  </si>
-  <si>
-    <t>초월 유전자는 부모 모두가 공유할 때만 유전될 수 있습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>초월 유전자는 유전됩니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>변형인자는 생식유전자와 함께 유전될 수 있습니다.</t>
-  </si>
-  <si>
-    <t>- Better Gene Inheritance -</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -160,7 +106,80 @@
         <color rgb="FF000000"/>
         <rFont val="맑은 고딕"/>
         <family val="3"/>
-        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>초월 유전자는 부모 모두가 공유할 때만 유전될 수 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>BGI_InheritArchite</t>
+  </si>
+  <si>
+    <t>Archite Genes are inheritable.</t>
+  </si>
+  <si>
+    <t>Keyed+BGI_InheritXeno</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>초월 유전자는 유전됩니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>BGI_InheritXeno</t>
+  </si>
+  <si>
+    <t>Xenogenes can be inherited along with the endogenes.</t>
+  </si>
+  <si>
+    <t>변형인자는 생식유전자와 함께 유전될 수 있습니다.</t>
+  </si>
+  <si>
+    <t>Keyed+BGInheritance</t>
+  </si>
+  <si>
+    <t>BGInheritance</t>
+  </si>
+  <si>
+    <t>Better Gene Inheritance</t>
+  </si>
+  <si>
+    <t>Keyed+BGI_MetabolismLimit</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Better Gene Inheritance -</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>BGI_MetabolismLimit</t>
+  </si>
+  <si>
+    <t>Lowest permitted metabolism</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
       </rPr>
       <t>최저</t>
     </r>
@@ -179,7 +198,6 @@
         <color rgb="FF000000"/>
         <rFont val="맑은 고딕"/>
         <family val="3"/>
-        <charset val="129"/>
       </rPr>
       <t>허용</t>
     </r>
@@ -198,10 +216,92 @@
         <color rgb="FF000000"/>
         <rFont val="맑은 고딕"/>
         <family val="3"/>
-        <charset val="129"/>
       </rPr>
       <t>대사</t>
     </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>GeneDef+BGI_BinaryInheritance.label</t>
+  </si>
+  <si>
+    <t>BGI_BinaryInheritance.label</t>
+  </si>
+  <si>
+    <t>Binary Inheritance</t>
+  </si>
+  <si>
+    <t>GeneDef+BGI_BinaryInheritance.description</t>
+  </si>
+  <si>
+    <t>BGI_BinaryInheritance.description</t>
+  </si>
+  <si>
+    <t>If both the carrier of this gene AND their partner have this gene then a full geneset will be picked from one parent or the other.\n\nThis gene is commonly found among xenotypes with castes or extreme sexual dimorphism.\n\nThis can be combined with dominant/recessive genes, which, if so, will take precedence over this gene.</t>
+  </si>
+  <si>
+    <t>GeneDef+BGI_PrimaryGenes.label</t>
+  </si>
+  <si>
+    <t>BGI_PrimaryGenes.label</t>
+  </si>
+  <si>
+    <t>Primary Genes</t>
+  </si>
+  <si>
+    <t>GeneDef+BGI_PrimaryGenes.description</t>
+  </si>
+  <si>
+    <t>BGI_PrimaryGenes.description</t>
+  </si>
+  <si>
+    <t>Carriers of this gene will have their genes be more prevalent in their offspring, especially when mixed with a baseliner.\n\nThis means they will usually pass down all their genes unless they conflict with those of the other parent.</t>
+  </si>
+  <si>
+    <t>GeneDef+BGI_SecondaryGenes.label</t>
+  </si>
+  <si>
+    <t>BGI_SecondaryGenes.label</t>
+  </si>
+  <si>
+    <t>Secondary Genes</t>
+  </si>
+  <si>
+    <t>GeneDef+BGI_SecondaryGenes.description</t>
+  </si>
+  <si>
+    <t>BGI_SecondaryGenes.description</t>
+  </si>
+  <si>
+    <t>Carriers of this gene will have their genes be less prevalent in their offspring.\n\nhis means the other parent will usually pass down all their genes unless there is a conflict.</t>
+  </si>
+  <si>
+    <t>이진 유전</t>
+  </si>
+  <si>
+    <t>주 유전자</t>
+  </si>
+  <si>
+    <t>부 유전자</t>
+  </si>
+  <si>
+    <t>이 유전자의 보유자와 그 파트너 모두가 이 유전자를 가지고 있다면, 전체 유전자 세트는 한 부모 또는 다른 부모 중에서 선택됩니다.\n\n이 유전자는 카스트나 극단적인 성적 이형성증을 가진 제노타입에서 일반적으로 발견됩니다.\n\n이 유전자는 우성/열성 유전자와 결합할 수 있으며, 이 경우 우성/열성 유전자가 이 유전자보다 우선합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 자손에서 유전자가 더 많이 나타납니다. 특히 일반인과 혼합될 때 그렇습니다.\n\n이는 다른 부모의 유전자와 충돌하지 않는 한, 일반적으로 모든 유전자를 전달한다는 것을 의미합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자의 보유자는 자손에서 유전자가 덜 나타납니다.\n\n이는 다른 부모가 모든 유전자를 전달하며, 충돌이 없는 한 그렇게 된다는 것을 의미합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자를 가진 사람은 자손에게 모든 유전자를 전달하며, 파트너의 유전자는 무시됩니다. 단, 파트너도 이 유전자를 가진 경우는 예외입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 유전자를 가진 사람은 자손에게 아무 유전자도 전달하지 않으며, 파트너의 유전자만 받습니다. 단, 파트너도 이 유전자를 가진 경우는 예외입니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -209,7 +309,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -238,17 +338,23 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
-      <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -271,12 +377,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -579,13 +686,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" style="1" customWidth="1"/>
@@ -629,144 +736,246 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>35</v>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>